<commit_message>
Added info and metadata to FCF download/upload
</commit_message>
<xml_diff>
--- a/public/sample_uploads/form_custom_fields.xlsx
+++ b/public/sample_uploads/form_custom_fields.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">Field Type</t>
   </si>
   <si>
+    <t xml:space="preserve">Metadata</t>
+  </si>
+  <si>
     <t xml:space="preserve">Required</t>
   </si>
   <si>
@@ -40,6 +43,9 @@
     <t xml:space="preserve">Position</t>
   </si>
   <si>
+    <t xml:space="preserve">Info</t>
+  </si>
+  <si>
     <t xml:space="preserve">Help Text</t>
   </si>
   <si>
@@ -97,6 +103,12 @@
     <t xml:space="preserve">Select</t>
   </si>
   <si>
+    <t xml:space="preserve">Domestic,Foreign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is for foreign remittances</t>
+  </si>
+  <si>
     <t xml:space="preserve">entity_type</t>
   </si>
   <si>
@@ -107,6 +119,9 @@
   </si>
   <si>
     <t xml:space="preserve">constitution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A,B,C</t>
   </si>
   <si>
     <t xml:space="preserve">address</t>
@@ -363,10 +378,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P15" activeCellId="0" sqref="P15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.47265625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -374,21 +389,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="95.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="25.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="22.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="21.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="13.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="13.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="95.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="25.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="22.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="21.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16380" min="16380" style="0" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16381" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="21.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16382" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -440,559 +454,597 @@
       <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
-        <v>18</v>
+      <c r="J2" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P2" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
-        <v>18</v>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P3" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="E4" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="H4" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
-        <v>18</v>
+      <c r="J4" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="2" t="s">
-        <v>18</v>
+      <c r="J5" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O5" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P5" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="R5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
-        <v>18</v>
+      <c r="J6" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P6" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q6" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="R6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="E7" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>18</v>
+      <c r="J7" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O7" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="R7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>18</v>
+      <c r="J8" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O8" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P8" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
-        <v>18</v>
+      <c r="J9" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O9" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P9" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q9" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2" t="s">
-        <v>18</v>
+      <c r="J10" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O10" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P10" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q10" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
-        <v>18</v>
+      <c r="J11" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O11" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q11" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2" t="s">
-        <v>18</v>
+      <c r="J12" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O12" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P12" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q12" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2" t="s">
-        <v>18</v>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O13" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="P13" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q13" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="R13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+      <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
-        <v>18</v>
+      <c r="J14" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O14" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="O14" s="2"/>
       <c r="P14" s="2" t="s">
-        <v>38</v>
+        <v>22</v>
+      </c>
+      <c r="Q14" s="3" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>